<commit_message>
Define Excel pattern functions
This is initial attempts to extract the Excel sheet values and convert them to OWL classes.
</commit_message>
<xml_diff>
--- a/dev-resources/xls-test.xlsx
+++ b/dev-resources/xls-test.xlsx
@@ -5,28 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aisha\Desktop\tawny-bubo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aisha\Desktop\tawny-bubo\dev-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D746D9C9-BB00-4536-9B6C-057D02E598FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB4A97D-BC97-425F-B396-D71B0131B18B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -55,32 +63,103 @@
     <t>B2</t>
   </si>
   <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>A22</t>
-  </si>
-  <si>
-    <t>r11</t>
-  </si>
-  <si>
-    <t>r22</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>B22</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>1 0 AM</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>www.10am.bandcamp.com/</t>
+  </si>
+  <si>
+    <t>Alice Ella</t>
+  </si>
+  <si>
+    <t>www.aliceella.co.uk</t>
+  </si>
+  <si>
+    <t>Alina Bzhezhinska</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>www.alina-harpist.com</t>
+  </si>
+  <si>
+    <t>Alison Beattie</t>
+  </si>
+  <si>
+    <t>Classical</t>
+  </si>
+  <si>
+    <t>www.alisonbeattiemusic.com</t>
+  </si>
+  <si>
+    <t>www.alisonrayner.com</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>Y3</t>
+  </si>
+  <si>
+    <t>Alison Rayner</t>
+  </si>
+  <si>
+    <t>Artists/Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,8 +185,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,48 +517,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8708DBD-178D-4F0D-98E3-DC8CEA339F61}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96F145A-23CB-40F7-B53F-DAB598D14BE3}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25CB53E-4BEE-4E5A-9377-8190D172771C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove spaces and characters from class name
</commit_message>
<xml_diff>
--- a/dev-resources/xls-test.xlsx
+++ b/dev-resources/xls-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aisha\Desktop\tawny-bubo\dev-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB4A97D-BC97-425F-B396-D71B0131B18B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89E4267-23B3-452F-BFAA-E205F9EF5E40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1770" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,67 +517,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8708DBD-178D-4F0D-98E3-DC8CEA339F61}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -590,7 +578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96F145A-23CB-40F7-B53F-DAB598D14BE3}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>